<commit_message>
fix(lib): Update lt-nis2-kibernetinio-saugumo-istatymas.xlsx (#2509)
Update lt-nis2-kibernetinio-saugumo-istatymas.xlsx

remove remote dependency
</commit_message>
<xml_diff>
--- a/tools/excel/lt-nis2-kibernetinio-saugumo-istatymas/lt-nis2-kibernetinio-saugumo-istatymas.xlsx
+++ b/tools/excel/lt-nis2-kibernetinio-saugumo-istatymas/lt-nis2-kibernetinio-saugumo-istatymas.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileSharing readOnlyRecommended="1"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/git/work-mkt/ciso-assistant-community/tools/excel/lt-nis2-kibernetinio-saugumo-istatymas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/excel/lt-nis2-kibernetinio-saugumo-istatymas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2676F5A-3897-6641-B4A3-7AB677FBD7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C186D424-8F4A-9C4A-9991-FA0B0082C573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="760" windowWidth="29000" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -20,6 +21,7 @@
     <sheet name="implementation_groups_content" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">req_content!$A$1:$F$216</definedName>
     <definedName name="requirement_nodes_1" localSheetId="2">req_content!$A$1:$F$294</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -28,7 +30,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{5483511E-034D-0C44-95C3-18CA4ABE7590}" name="requirement_nodes" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="1" xr16:uid="{5483511E-034D-0C44-95C3-18CA4ABE7590}" name="requirement_nodes" type="6" refreshedVersion="8" deleted="1" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="/Users/macbook/git/work-mkt/ciso-assistant-community/requirement_nodes.csv" tab="0" comma="1">
       <textFields count="7">
         <textField type="text"/>
@@ -2524,11 +2526,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="110" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2619,11 +2625,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="173" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="108.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2690,15 +2699,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F295"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="161" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.5" customWidth="1"/>
     <col min="5" max="5" width="43.33203125" style="4" customWidth="1"/>
     <col min="6" max="6" width="80.6640625" style="4" bestFit="1" customWidth="1"/>
@@ -7324,6 +7333,7 @@
       <c r="F295" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F216" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -7338,6 +7348,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -7364,7 +7377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047D0A24-116B-B54F-99CA-DF252F5EFFFF}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="184" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>